<commit_message>
Updated PCA and LDA datasets for all cases
</commit_message>
<xml_diff>
--- a/data/mixture/8 solutions/PCA_without_112_121.xlsx
+++ b/data/mixture/8 solutions/PCA_without_112_121.xlsx
@@ -1107,7 +1107,11 @@
       <c r="B52" t="n">
         <v>169.2180388386178</v>
       </c>
-      <c r="C52" t="inlineStr"/>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Mix_211</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -1116,7 +1120,11 @@
       <c r="B53" t="n">
         <v>128.578683108253</v>
       </c>
-      <c r="C53" t="inlineStr"/>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Mix_211</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -1125,7 +1133,11 @@
       <c r="B54" t="n">
         <v>115.1937857700003</v>
       </c>
-      <c r="C54" t="inlineStr"/>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Mix_211</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -1134,7 +1146,11 @@
       <c r="B55" t="n">
         <v>-213.7732925055967</v>
       </c>
-      <c r="C55" t="inlineStr"/>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Mix_211</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -1143,7 +1159,11 @@
       <c r="B56" t="n">
         <v>-191.8385891760132</v>
       </c>
-      <c r="C56" t="inlineStr"/>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Mix_211</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -1152,7 +1172,11 @@
       <c r="B57" t="n">
         <v>-192.7085903196967</v>
       </c>
-      <c r="C57" t="inlineStr"/>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Mix_211</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -1161,7 +1185,11 @@
       <c r="B58" t="n">
         <v>-194.9192262477846</v>
       </c>
-      <c r="C58" t="inlineStr"/>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Mix_211</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -1170,7 +1198,11 @@
       <c r="B59" t="n">
         <v>-150.3960632355945</v>
       </c>
-      <c r="C59" t="inlineStr"/>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Mix_211</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -1179,7 +1211,11 @@
       <c r="B60" t="n">
         <v>-144.3151470013213</v>
       </c>
-      <c r="C60" t="inlineStr"/>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Mix_211</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -1188,7 +1224,11 @@
       <c r="B61" t="n">
         <v>-108.4941777150933</v>
       </c>
-      <c r="C61" t="inlineStr"/>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Mix_211</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>